<commit_message>
Reoredered legs and added function and controls to detailed leg control
</commit_message>
<xml_diff>
--- a/New_UI.xlsx
+++ b/New_UI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://peterru-my.sharepoint.com/personal/me_peterrusiecki_eu/Documents/Code/hexapod_code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="940" documentId="8_{66BD43C0-C38C-4CBA-8B7E-386B1F07CDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89878F54-4D55-4B1B-8EBE-214D56543E8B}"/>
+  <xr:revisionPtr revIDLastSave="954" documentId="8_{66BD43C0-C38C-4CBA-8B7E-386B1F07CDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{127F5B88-95E4-4B79-8EC4-2D8D8203D684}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{EE134321-7F2B-40EB-98BD-7232E33EDF77}"/>
+    <workbookView xWindow="5715" yWindow="0" windowWidth="18585" windowHeight="10350" xr2:uid="{EE134321-7F2B-40EB-98BD-7232E33EDF77}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
   <si>
     <t>Old Button</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Refresh</t>
+  </si>
+  <si>
+    <t>Update</t>
   </si>
 </sst>
 </file>
@@ -1030,6 +1033,15 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1052,15 +1064,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1141,13 +1144,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1506,10 +1509,10 @@
   <dimension ref="A1:CW51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AL5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BC23" sqref="BC23:BF23"/>
+      <selection pane="bottomRight" activeCell="BM28" sqref="BM28:BM29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.9296875" defaultRowHeight="10.050000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2488,7 +2491,7 @@
       <c r="AS10" s="3"/>
       <c r="AT10" s="5"/>
       <c r="AU10" s="42" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="AV10" s="43"/>
       <c r="AW10" s="46"/>
@@ -2511,7 +2514,7 @@
       <c r="BJ10" s="46"/>
       <c r="BK10" s="3"/>
       <c r="BL10" s="42" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="BM10" s="43"/>
       <c r="BN10" s="46"/>
@@ -2693,9 +2696,9 @@
       <c r="BQ12" s="3"/>
       <c r="BR12" s="3"/>
       <c r="BS12" s="3"/>
-      <c r="BV12" s="91"/>
-      <c r="BW12" s="91"/>
-      <c r="BX12" s="91"/>
+      <c r="BV12" s="93"/>
+      <c r="BW12" s="93"/>
+      <c r="BX12" s="93"/>
       <c r="CE12" s="2" t="s">
         <v>35</v>
       </c>
@@ -3304,7 +3307,7 @@
       <c r="AQ19" s="3"/>
       <c r="AR19" s="7"/>
       <c r="AS19" s="42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AT19" s="43"/>
       <c r="AU19" s="46"/>
@@ -3327,7 +3330,7 @@
       <c r="BL19" s="3"/>
       <c r="BM19" s="3"/>
       <c r="BN19" s="42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="BO19" s="43"/>
       <c r="BP19" s="46"/>
@@ -3568,10 +3571,12 @@
       <c r="AZ22" s="43"/>
       <c r="BA22" s="53"/>
       <c r="BB22" s="6"/>
-      <c r="BC22" s="3"/>
-      <c r="BD22" s="3"/>
-      <c r="BE22" s="3"/>
-      <c r="BF22" s="3"/>
+      <c r="BC22" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="BD22" s="55"/>
+      <c r="BE22" s="55"/>
+      <c r="BF22" s="56"/>
       <c r="BG22" s="5"/>
       <c r="BH22" s="53"/>
       <c r="BI22" s="43" t="s">
@@ -3657,12 +3662,12 @@
         <v>56</v>
       </c>
       <c r="BB23" s="6"/>
-      <c r="BC23" s="62" t="s">
+      <c r="BC23" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="BD23" s="63"/>
-      <c r="BE23" s="63"/>
-      <c r="BF23" s="64"/>
+      <c r="BD23" s="55"/>
+      <c r="BE23" s="55"/>
+      <c r="BF23" s="56"/>
       <c r="BG23" s="5"/>
       <c r="BH23" s="52" t="s">
         <v>56</v>
@@ -4070,14 +4075,14 @@
       <c r="AY28" s="3"/>
       <c r="AZ28" s="3"/>
       <c r="BA28" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BB28" s="43"/>
       <c r="BC28" s="46"/>
       <c r="BD28" s="3"/>
       <c r="BE28" s="3"/>
       <c r="BF28" s="42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BG28" s="43"/>
       <c r="BH28" s="46"/>
@@ -5086,14 +5091,14 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="5"/>
-      <c r="J42" s="92" t="s">
+      <c r="J42" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="K42" s="93"/>
-      <c r="L42" s="92" t="s">
+      <c r="K42" s="92"/>
+      <c r="L42" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="M42" s="93"/>
+      <c r="M42" s="92"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
@@ -5574,14 +5579,14 @@
       <c r="G48" s="38"/>
       <c r="H48" s="38"/>
       <c r="I48" s="5"/>
-      <c r="J48" s="54" t="s">
+      <c r="J48" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="K48" s="55"/>
-      <c r="L48" s="55"/>
-      <c r="M48" s="55"/>
-      <c r="N48" s="55"/>
-      <c r="O48" s="56"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="58"/>
+      <c r="O48" s="59"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="38" t="s">
         <v>22</v>
@@ -5603,14 +5608,14 @@
       <c r="AD48" s="38"/>
       <c r="AE48" s="3"/>
       <c r="AF48" s="3"/>
-      <c r="AG48" s="62" t="s">
+      <c r="AG48" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="AH48" s="63"/>
-      <c r="AI48" s="63"/>
-      <c r="AJ48" s="63"/>
-      <c r="AK48" s="63"/>
-      <c r="AL48" s="64"/>
+      <c r="AH48" s="55"/>
+      <c r="AI48" s="55"/>
+      <c r="AJ48" s="55"/>
+      <c r="AK48" s="55"/>
+      <c r="AL48" s="56"/>
       <c r="AM48" s="3"/>
       <c r="AN48" s="38" t="s">
         <v>20</v>
@@ -5645,12 +5650,12 @@
       <c r="BJ48" s="38"/>
       <c r="BK48" s="38"/>
       <c r="BL48" s="3"/>
-      <c r="BM48" s="59"/>
-      <c r="BN48" s="60"/>
-      <c r="BO48" s="60"/>
-      <c r="BP48" s="60"/>
-      <c r="BQ48" s="60"/>
-      <c r="BR48" s="61"/>
+      <c r="BM48" s="62"/>
+      <c r="BN48" s="63"/>
+      <c r="BO48" s="63"/>
+      <c r="BP48" s="63"/>
+      <c r="BQ48" s="63"/>
+      <c r="BR48" s="64"/>
       <c r="BS48" s="3"/>
     </row>
     <row r="49" spans="1:71" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5769,23 +5774,23 @@
       <c r="AD50" s="38"/>
       <c r="AE50" s="3"/>
       <c r="AF50" s="3"/>
-      <c r="AG50" s="62" t="s">
+      <c r="AG50" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="AH50" s="63"/>
-      <c r="AI50" s="63"/>
-      <c r="AJ50" s="63"/>
-      <c r="AK50" s="63"/>
-      <c r="AL50" s="64"/>
+      <c r="AH50" s="55"/>
+      <c r="AI50" s="55"/>
+      <c r="AJ50" s="55"/>
+      <c r="AK50" s="55"/>
+      <c r="AL50" s="56"/>
       <c r="AM50" s="3"/>
-      <c r="AN50" s="54" t="s">
+      <c r="AN50" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="AO50" s="55"/>
-      <c r="AP50" s="55"/>
-      <c r="AQ50" s="55"/>
-      <c r="AR50" s="55"/>
-      <c r="AS50" s="56"/>
+      <c r="AO50" s="58"/>
+      <c r="AP50" s="58"/>
+      <c r="AQ50" s="58"/>
+      <c r="AR50" s="58"/>
+      <c r="AS50" s="59"/>
       <c r="AT50" s="3"/>
       <c r="AU50" s="38" t="s">
         <v>16</v>
@@ -5811,11 +5816,11 @@
       <c r="BJ50" s="38"/>
       <c r="BK50" s="38"/>
       <c r="BL50" s="3"/>
-      <c r="BM50" s="57"/>
-      <c r="BN50" s="58"/>
-      <c r="BO50" s="58"/>
-      <c r="BP50" s="58"/>
-      <c r="BQ50" s="58"/>
+      <c r="BM50" s="60"/>
+      <c r="BN50" s="61"/>
+      <c r="BO50" s="61"/>
+      <c r="BP50" s="61"/>
+      <c r="BQ50" s="61"/>
       <c r="BR50" s="51"/>
       <c r="BS50" s="3"/>
     </row>
@@ -5895,7 +5900,7 @@
       <c r="BS51" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="107">
+  <mergeCells count="108">
     <mergeCell ref="AT5:AU6"/>
     <mergeCell ref="BK42:BN42"/>
     <mergeCell ref="AU42:AX42"/>
@@ -5912,6 +5917,14 @@
     <mergeCell ref="BM6:BM7"/>
     <mergeCell ref="BJ6:BK7"/>
     <mergeCell ref="AX6:AY7"/>
+    <mergeCell ref="AR17:AS17"/>
+    <mergeCell ref="AV16:AW16"/>
+    <mergeCell ref="AZ17:BA17"/>
+    <mergeCell ref="BF17:BG17"/>
+    <mergeCell ref="BJ16:BK16"/>
+    <mergeCell ref="AT17:AU17"/>
+    <mergeCell ref="AS15:AT16"/>
+    <mergeCell ref="BM28:BM29"/>
     <mergeCell ref="BK43:BN43"/>
     <mergeCell ref="AU43:AX43"/>
     <mergeCell ref="AR32:BA41"/>
@@ -5948,14 +5961,6 @@
     <mergeCell ref="AU48:AZ48"/>
     <mergeCell ref="AU50:AZ50"/>
     <mergeCell ref="AG48:AL48"/>
-    <mergeCell ref="AR17:AS17"/>
-    <mergeCell ref="AV16:AW16"/>
-    <mergeCell ref="AZ17:BA17"/>
-    <mergeCell ref="BF17:BG17"/>
-    <mergeCell ref="BJ16:BK16"/>
-    <mergeCell ref="AT17:AU17"/>
-    <mergeCell ref="AS15:AT16"/>
-    <mergeCell ref="BM28:BM29"/>
     <mergeCell ref="BH23:BH24"/>
     <mergeCell ref="AV28:AV29"/>
     <mergeCell ref="BA23:BA24"/>
@@ -5966,6 +5971,7 @@
     <mergeCell ref="BH21:BH22"/>
     <mergeCell ref="AW25:AX25"/>
     <mergeCell ref="BI25:BJ25"/>
+    <mergeCell ref="BC22:BF22"/>
     <mergeCell ref="AY8:AZ8"/>
     <mergeCell ref="BK8:BL8"/>
     <mergeCell ref="AX16:AY16"/>
@@ -7248,6 +7254,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C11:F11"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="X3:AJ15"/>
@@ -7263,8 +7271,6 @@
     <mergeCell ref="S19:U19"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>